<commit_message>
Version 2.0 PixelBot application
</commit_message>
<xml_diff>
--- a/TaggingRequest_2021.xlsx
+++ b/TaggingRequest_2021.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albeiro.jimenez\Documents\Xaxis_Projects\tagCalc\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albeiro.jimenez\Documents\Xaxis_Projects\tagCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B6810D-865B-4907-817A-20F8D6798466}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FC6CA9-B9DA-4892-8209-14D75F08A92C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,9 +123,6 @@
     <t>Anunciante</t>
   </si>
   <si>
-    <t>OlxAutos</t>
-  </si>
-  <si>
     <t>Campaña</t>
   </si>
   <si>
@@ -463,6 +460,9 @@
   </si>
   <si>
     <t>Convertion</t>
+  </si>
+  <si>
+    <t>Xaxis</t>
   </si>
 </sst>
 </file>
@@ -694,6 +694,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -706,27 +721,12 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1342,8 +1342,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A18:AMJ136"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2427,7 +2427,7 @@
   <dimension ref="A11:AMI315"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2464,12 +2464,12 @@
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="4"/>
     </row>
@@ -2478,128 +2478,128 @@
     </row>
     <row r="16" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="4"/>
     </row>
     <row r="22" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="4"/>
     </row>
     <row r="23" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="7"/>
     </row>
     <row r="27" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J28" s="23" t="s">
+      <c r="J28" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="21"/>
+    </row>
+    <row r="29" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K28" s="23"/>
-    </row>
-    <row r="29" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="24" t="s">
+      <c r="C29" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="D29" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="E29" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="F29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="G29" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="H29" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="24" t="s">
+      <c r="I29" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="24" t="s">
+      <c r="J29" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="J29" s="25" t="s">
+      <c r="K29" s="18"/>
+      <c r="L29" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="K29" s="25"/>
-      <c r="L29" s="22" t="s">
+      <c r="M29" s="19"/>
+    </row>
+    <row r="30" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M29" s="22"/>
-    </row>
-    <row r="30" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="3" t="s">
+      <c r="K30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K30" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="L30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M30" s="3" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="31" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="17" t="s">
-        <v>114</v>
+      <c r="B31" s="22" t="s">
+        <v>113</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -2610,11 +2610,11 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
     </row>
     <row r="32" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="18"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -2624,11 +2624,11 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="21"/>
-    </row>
-    <row r="33" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="19"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+    </row>
+    <row r="33" spans="2:13" s="8" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="24"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -2638,12 +2638,12 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
     </row>
     <row r="34" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="17" t="s">
-        <v>115</v>
+      <c r="B34" s="22" t="s">
+        <v>114</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -2654,11 +2654,11 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="21"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
     </row>
     <row r="35" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="20"/>
+      <c r="B35" s="25"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -2671,8 +2671,8 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
     </row>
-    <row r="36" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="20"/>
+    <row r="36" spans="2:13" s="8" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="25"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -2685,8 +2685,8 @@
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
     </row>
-    <row r="37" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="20"/>
+    <row r="37" spans="2:13" s="8" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="25"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -2699,8 +2699,8 @@
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
     </row>
-    <row r="38" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="20"/>
+    <row r="38" spans="2:13" s="8" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="25"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -2713,8 +2713,8 @@
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
     </row>
-    <row r="39" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="18"/>
+    <row r="39" spans="2:13" s="8" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="23"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -2724,11 +2724,11 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="21"/>
-    </row>
-    <row r="40" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="18"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+    </row>
+    <row r="40" spans="2:13" s="8" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="23"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -2738,11 +2738,11 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="21"/>
-      <c r="M40" s="21"/>
-    </row>
-    <row r="41" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="18"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+    </row>
+    <row r="41" spans="2:13" s="8" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="23"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -2752,11 +2752,11 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="21"/>
-      <c r="M41" s="21"/>
-    </row>
-    <row r="42" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="19"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+    </row>
+    <row r="42" spans="2:13" s="8" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="24"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -2766,12 +2766,12 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-      <c r="L42" s="21"/>
-      <c r="M42" s="21"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
     </row>
     <row r="43" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="17" t="s">
-        <v>116</v>
+      <c r="B43" s="22" t="s">
+        <v>115</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -2785,8 +2785,8 @@
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
     </row>
-    <row r="44" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="20"/>
+    <row r="44" spans="2:13" s="8" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="25"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -2799,8 +2799,8 @@
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
     </row>
-    <row r="45" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="20"/>
+    <row r="45" spans="2:13" s="8" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="25"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -2813,8 +2813,8 @@
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
     </row>
-    <row r="46" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="18"/>
+    <row r="46" spans="2:13" s="8" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="23"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -2827,8 +2827,8 @@
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
     </row>
-    <row r="47" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="18"/>
+    <row r="47" spans="2:13" s="8" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="23"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -2838,11 +2838,11 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
-      <c r="L47" s="21"/>
-      <c r="M47" s="21"/>
-    </row>
-    <row r="48" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="19"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="20"/>
+    </row>
+    <row r="48" spans="2:13" s="8" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="24"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -2852,8 +2852,8 @@
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
-      <c r="L48" s="21"/>
-      <c r="M48" s="21"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
     </row>
     <row r="49" spans="6:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F49" s="10"/>
@@ -3126,20 +3126,6 @@
     <row r="315" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="J28:K28"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B34:B42"/>
     <mergeCell ref="B43:B48"/>
@@ -3150,6 +3136,20 @@
     <mergeCell ref="L42:M42"/>
     <mergeCell ref="L47:M47"/>
     <mergeCell ref="L48:M48"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3162,8 +3162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0704531C-E89D-482F-A691-8949287AF91E}">
   <dimension ref="A11:AMI315"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M31" sqref="M31:M48"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3200,12 +3200,12 @@
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="4"/>
     </row>
@@ -3214,378 +3214,378 @@
     </row>
     <row r="16" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="4"/>
     </row>
     <row r="22" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="4"/>
     </row>
     <row r="23" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="7"/>
     </row>
     <row r="27" spans="2:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="2:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J28" s="23" t="s">
+      <c r="J28" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="21"/>
+    </row>
+    <row r="29" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K28" s="23"/>
-    </row>
-    <row r="29" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="24" t="s">
+      <c r="C29" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="D29" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="E29" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="F29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="G29" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="H29" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="24" t="s">
+      <c r="I29" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="24" t="s">
+      <c r="J29" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="J29" s="25" t="s">
+      <c r="K29" s="18"/>
+      <c r="L29" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="K29" s="25"/>
-      <c r="L29" s="22" t="s">
+      <c r="M29" s="19"/>
+    </row>
+    <row r="30" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M29" s="22"/>
-    </row>
-    <row r="30" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="3" t="s">
+      <c r="K30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K30" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="L30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M30" s="3" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="31" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
+      <c r="B31" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
     </row>
     <row r="32" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="26"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="27"/>
     </row>
     <row r="33" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="26"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="27"/>
     </row>
     <row r="34" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="26"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="28"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="27"/>
     </row>
     <row r="35" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="26"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="28"/>
-      <c r="L35" s="28"/>
-      <c r="M35" s="28"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
+      <c r="L35" s="27"/>
+      <c r="M35" s="27"/>
     </row>
     <row r="36" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="26"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="28"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
-      <c r="K36" s="28"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="28"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
     </row>
     <row r="37" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="26"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="28"/>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="28"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
     </row>
     <row r="38" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="26"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="28"/>
-      <c r="K38" s="28"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="28"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
     </row>
     <row r="39" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="26"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="28"/>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="28"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
     </row>
     <row r="40" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="26"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="28"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
     </row>
     <row r="41" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="26"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28"/>
-      <c r="M41" s="28"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="27"/>
     </row>
     <row r="42" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="26"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="28"/>
-      <c r="L42" s="28"/>
-      <c r="M42" s="28"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="27"/>
     </row>
     <row r="43" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="26"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="28"/>
-      <c r="K43" s="28"/>
-      <c r="L43" s="28"/>
-      <c r="M43" s="28"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="27"/>
     </row>
     <row r="44" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="26"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="28"/>
-      <c r="J44" s="28"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="28"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="27"/>
     </row>
     <row r="45" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="26"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="28"/>
-      <c r="K45" s="28"/>
-      <c r="L45" s="28"/>
-      <c r="M45" s="28"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
     </row>
     <row r="46" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="26"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="28"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="28"/>
-      <c r="M46" s="28"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="27"/>
+      <c r="M46" s="27"/>
     </row>
     <row r="47" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="26"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="28"/>
-      <c r="K47" s="28"/>
-      <c r="L47" s="28"/>
-      <c r="M47" s="28"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="27"/>
+      <c r="K47" s="27"/>
+      <c r="L47" s="27"/>
+      <c r="M47" s="27"/>
     </row>
     <row r="48" spans="2:13" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="26"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="29"/>
-      <c r="H48" s="29"/>
-      <c r="I48" s="29"/>
-      <c r="J48" s="29"/>
-      <c r="K48" s="29"/>
-      <c r="L48" s="29"/>
-      <c r="M48" s="29"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="28"/>
+      <c r="J48" s="28"/>
+      <c r="K48" s="28"/>
+      <c r="L48" s="28"/>
+      <c r="M48" s="28"/>
     </row>
     <row r="49" spans="6:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F49" s="10"/>
@@ -3858,16 +3858,6 @@
     <row r="315" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="I31:I48"/>
-    <mergeCell ref="J31:J48"/>
-    <mergeCell ref="K31:K48"/>
-    <mergeCell ref="L31:L48"/>
-    <mergeCell ref="M31:M48"/>
-    <mergeCell ref="B31:B48"/>
-    <mergeCell ref="C31:C48"/>
-    <mergeCell ref="D31:D48"/>
-    <mergeCell ref="E31:E48"/>
-    <mergeCell ref="G31:G48"/>
     <mergeCell ref="H31:H48"/>
     <mergeCell ref="L29:M29"/>
     <mergeCell ref="J28:K28"/>
@@ -3880,6 +3870,16 @@
     <mergeCell ref="H29:H30"/>
     <mergeCell ref="I29:I30"/>
     <mergeCell ref="J29:K29"/>
+    <mergeCell ref="B31:B48"/>
+    <mergeCell ref="C31:C48"/>
+    <mergeCell ref="D31:D48"/>
+    <mergeCell ref="E31:E48"/>
+    <mergeCell ref="G31:G48"/>
+    <mergeCell ref="I31:I48"/>
+    <mergeCell ref="J31:J48"/>
+    <mergeCell ref="K31:K48"/>
+    <mergeCell ref="L31:L48"/>
+    <mergeCell ref="M31:M48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3913,85 +3913,85 @@
     </row>
     <row r="4" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="14" t="s">
+      <c r="I4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="13"/>
       <c r="D5" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="13"/>
       <c r="D6" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="13"/>
       <c r="D7" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="12"/>
       <c r="F8" s="13"/>
       <c r="G8" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="12"/>
       <c r="F9" s="13"/>
       <c r="G9" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="13" t="s">
         <v>43</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4000,104 +4000,104 @@
     </row>
     <row r="11" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="F11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="14" t="s">
+      <c r="I11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="13" t="s">
+      <c r="L11" s="13" t="s">
         <v>48</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="13"/>
       <c r="D12" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="13"/>
       <c r="D13" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K13" s="13"/>
       <c r="L13" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="13"/>
       <c r="D14" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="L14" s="13" t="s">
         <v>57</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="13"/>
       <c r="D15" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I15" s="13"/>
       <c r="J15" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="L15" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="13"/>
       <c r="D16" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I16" s="13"/>
       <c r="J16" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="13"/>
       <c r="D17" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4110,13 +4110,13 @@
       <c r="D20" s="12"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="H20" s="13" t="s">
-        <v>66</v>
-      </c>
       <c r="I20" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4124,230 +4124,230 @@
         <v>0</v>
       </c>
       <c r="D21" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="G21" s="13" t="s">
         <v>68</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>69</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="13"/>
       <c r="D22" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F22" s="13"/>
       <c r="G22" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H22" s="13"/>
       <c r="I22" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="13"/>
       <c r="D23" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H23" s="13"/>
       <c r="I23" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="13"/>
       <c r="D24" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H24" s="13"/>
       <c r="I24" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F25" s="13"/>
       <c r="G25" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H25" s="13"/>
       <c r="I25" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="12"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="15" t="s">
         <v>9</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>10</v>
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="13"/>
       <c r="D28" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="13"/>
       <c r="D29" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="G31" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="H31" s="11" t="s">
         <v>86</v>
-      </c>
-      <c r="H31" s="11" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="32" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G32" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H32" s="11" t="s">
         <v>88</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="33" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="G33" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="G33" s="11" t="s">
-        <v>92</v>
-      </c>
       <c r="H33" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="G34" s="11" t="s">
         <v>94</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="35" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="G35" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="36" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="37" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="38" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" s="11" t="s">
         <v>103</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="39" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E40" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E41" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E42" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E43" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="44" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C45" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>